<commit_message>
TEX> updated dataset section
</commit_message>
<xml_diff>
--- a/code/output/preprocessing/NNDL_MN10_SAMPLES_DISTRIBUITIONS.xlsx
+++ b/code/output/preprocessing/NNDL_MN10_SAMPLES_DISTRIBUITIONS.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harjo\Workspace\UniPD\repo\3d_classification\code\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harjo\Workspace\UniPD\repo\3d_classification\code\output\preprocessing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE856500-8D52-4FC4-B087-E48E45CFEEF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B236D3D-CB3F-45CE-85A4-567CB133861B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{EF987BAC-AB0D-4C32-BA9C-87D58BA3652C}"/>
   </bookViews>
@@ -2826,6 +2826,671 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="150" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>TEST Set</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="150" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Initial samples</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="narVert">
+              <a:fgClr>
+                <a:schemeClr val="accent1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="20000"/>
+                  <a:lumOff val="80000"/>
+                </a:schemeClr>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:innerShdw blurRad="114300">
+                <a:schemeClr val="accent1"/>
+              </a:innerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$15:$B$24</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>bathtub</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>bed</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>chair</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>desk</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>dresser</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>monitor</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>night_stand </c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>sofa</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>table</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>toilet</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$2:$C$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A783-4883-8E42-A1FB92DE8AC3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>AFTER AUGMENTING</c:v>
+                </c:pt>
+              </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="narVert">
+              <a:fgClr>
+                <a:schemeClr val="accent2"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="20000"/>
+                  <a:lumOff val="80000"/>
+                </a:schemeClr>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:innerShdw blurRad="114300">
+                <a:schemeClr val="accent2"/>
+              </a:innerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$15:$B$24</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>bathtub</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>bed</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>chair</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>desk</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>dresser</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>monitor</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>night_stand </c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>sofa</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>table</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>toilet</c:v>
+                </c:pt>
+              </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$2:$F$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>258</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>258</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>258</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>300</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-A783-4883-8E42-A1FB92DE8AC3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="227"/>
+        <c:overlap val="-48"/>
+        <c:axId val="740487312"/>
+        <c:axId val="740486480"/>
+        <c:extLst/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="740487312"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="740486480"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="740486480"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="740487312"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+      </c:dTable>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -3026,6 +3691,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
   <cs:axisTitle>
@@ -5059,6 +5764,525 @@
 </file>
 
 <file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="217">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="narVert">
+        <a:fgClr>
+          <a:schemeClr val="phClr"/>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:effectLst>
+        <a:innerShdw blurRad="114300">
+          <a:schemeClr val="phClr"/>
+        </a:innerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="narVert">
+        <a:fgClr>
+          <a:schemeClr val="phClr"/>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:effectLst>
+        <a:innerShdw blurRad="114300">
+          <a:schemeClr val="phClr"/>
+        </a:innerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1800" b="1" kern="1200" cap="all" spc="150" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="217">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5765,6 +6989,44 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>405740</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>59377</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>69272</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{45EC839D-27C5-4AFD-88F8-962F742CD7F5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -6067,8 +7329,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80A91CEE-8044-4606-8677-3A953E0E3C8C}">
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="77" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="F48" zoomScale="69" workbookViewId="0">
+      <selection activeCell="V53" sqref="V53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6114,7 +7376,7 @@
         <v>3</v>
       </c>
       <c r="F2">
-        <f t="shared" ref="F2:F11" si="0">E2*D2</f>
+        <f>E2*D2</f>
         <v>150</v>
       </c>
     </row>
@@ -6126,14 +7388,14 @@
         <v>100</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D11" si="1">C3</f>
+        <f>C3</f>
         <v>100</v>
       </c>
       <c r="E3">
         <v>3</v>
       </c>
       <c r="F3">
-        <f t="shared" si="0"/>
+        <f>E3*D3</f>
         <v>300</v>
       </c>
     </row>
@@ -6145,14 +7407,14 @@
         <v>100</v>
       </c>
       <c r="D4">
-        <f t="shared" si="1"/>
+        <f>C4</f>
         <v>100</v>
       </c>
       <c r="E4">
         <v>3</v>
       </c>
       <c r="F4">
-        <f t="shared" si="0"/>
+        <f>E4*D4</f>
         <v>300</v>
       </c>
     </row>
@@ -6164,14 +7426,14 @@
         <v>86</v>
       </c>
       <c r="D5">
-        <f t="shared" si="1"/>
+        <f>C5</f>
         <v>86</v>
       </c>
       <c r="E5">
         <v>3</v>
       </c>
       <c r="F5">
-        <f t="shared" si="0"/>
+        <f>E5*D5</f>
         <v>258</v>
       </c>
     </row>
@@ -6183,14 +7445,14 @@
         <v>86</v>
       </c>
       <c r="D6">
-        <f t="shared" si="1"/>
+        <f>C6</f>
         <v>86</v>
       </c>
       <c r="E6">
         <v>3</v>
       </c>
       <c r="F6">
-        <f t="shared" si="0"/>
+        <f>E6*D6</f>
         <v>258</v>
       </c>
     </row>
@@ -6202,14 +7464,14 @@
         <v>100</v>
       </c>
       <c r="D7">
-        <f t="shared" si="1"/>
+        <f>C7</f>
         <v>100</v>
       </c>
       <c r="E7">
         <v>3</v>
       </c>
       <c r="F7">
-        <f t="shared" si="0"/>
+        <f>E7*D7</f>
         <v>300</v>
       </c>
     </row>
@@ -6221,14 +7483,14 @@
         <v>86</v>
       </c>
       <c r="D8">
-        <f t="shared" si="1"/>
+        <f>C8</f>
         <v>86</v>
       </c>
       <c r="E8">
         <v>3</v>
       </c>
       <c r="F8">
-        <f t="shared" si="0"/>
+        <f>E8*D8</f>
         <v>258</v>
       </c>
     </row>
@@ -6240,14 +7502,14 @@
         <v>100</v>
       </c>
       <c r="D9">
-        <f t="shared" si="1"/>
+        <f>C9</f>
         <v>100</v>
       </c>
       <c r="E9">
         <v>3</v>
       </c>
       <c r="F9">
-        <f t="shared" si="0"/>
+        <f>E9*D9</f>
         <v>300</v>
       </c>
     </row>
@@ -6259,14 +7521,14 @@
         <v>100</v>
       </c>
       <c r="D10">
-        <f t="shared" si="1"/>
+        <f>C10</f>
         <v>100</v>
       </c>
       <c r="E10">
         <v>3</v>
       </c>
       <c r="F10">
-        <f t="shared" si="0"/>
+        <f>E10*D10</f>
         <v>300</v>
       </c>
     </row>
@@ -6278,14 +7540,14 @@
         <v>100</v>
       </c>
       <c r="D11">
-        <f t="shared" si="1"/>
+        <f>C11</f>
         <v>100</v>
       </c>
       <c r="E11">
         <v>3</v>
       </c>
       <c r="F11">
-        <f t="shared" si="0"/>
+        <f>E11*D11</f>
         <v>300</v>
       </c>
     </row>
@@ -6348,7 +7610,7 @@
         <v>2</v>
       </c>
       <c r="F16">
-        <f t="shared" ref="F16:F24" si="2">D16*E16</f>
+        <f>D16*E16</f>
         <v>1000</v>
       </c>
     </row>
@@ -6366,7 +7628,7 @@
         <v>2</v>
       </c>
       <c r="F17">
-        <f t="shared" si="2"/>
+        <f>D17*E17</f>
         <v>1000</v>
       </c>
     </row>
@@ -6384,7 +7646,7 @@
         <v>5</v>
       </c>
       <c r="F18">
-        <f t="shared" si="2"/>
+        <f>D18*E18</f>
         <v>1000</v>
       </c>
     </row>
@@ -6402,7 +7664,7 @@
         <v>5</v>
       </c>
       <c r="F19">
-        <f t="shared" si="2"/>
+        <f>D19*E19</f>
         <v>1000</v>
       </c>
     </row>
@@ -6420,7 +7682,7 @@
         <v>2</v>
       </c>
       <c r="F20">
-        <f t="shared" si="2"/>
+        <f>D20*E20</f>
         <v>930</v>
       </c>
     </row>
@@ -6438,7 +7700,7 @@
         <v>5</v>
       </c>
       <c r="F21">
-        <f t="shared" si="2"/>
+        <f>D21*E21</f>
         <v>1000</v>
       </c>
     </row>
@@ -6456,7 +7718,7 @@
         <v>2</v>
       </c>
       <c r="F22">
-        <f t="shared" si="2"/>
+        <f>D22*E22</f>
         <v>1000</v>
       </c>
     </row>
@@ -6474,7 +7736,7 @@
         <v>3</v>
       </c>
       <c r="F23">
-        <f t="shared" si="2"/>
+        <f>D23*E23</f>
         <v>1176</v>
       </c>
     </row>
@@ -6492,7 +7754,7 @@
         <v>3</v>
       </c>
       <c r="F24">
-        <f t="shared" si="2"/>
+        <f>D24*E24</f>
         <v>1032</v>
       </c>
     </row>

</xml_diff>